<commit_message>
Added NCATS Study comb testcases from 11to20
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_StudyNCATSCOP01-Breed_PrimDiseaseSite.xlsx
+++ b/InputFiles/TC01_Canine_StudyNCATSCOP01-Breed_PrimDiseaseSite.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0302\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C65FE38-21C6-4B66-99BB-55F292DAC36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9BA62E-4A87-4A61-A967-F34D44203D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -63,24 +63,54 @@
     <t>StudyFilesTab</t>
   </si>
   <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+    <t>TC01_Canine_StudyNCATSCOP01-Breed_PrimDiseaseSite_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC01_Canine_StudyNCATSCOP01-Breed_PrimDiseaseSite_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)
+MATCH (demo:demographic) 
+MATCH (diag:diagnosis)
+MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation IN ['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
+OPTIONAL MATCH (s)&lt;-[:member_of]-(c:case),(s:study)
+OPTIONAL MATCH (c)&lt;-[:of_case]-(samp:sample)
+OPTIONAL MATCH (cf:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+RETURN  
+count(distinct p) AS Programs,
+count(distinct s) AS Studies,
+count(distinct c) AS Cases,
+count(distinct samp) AS Samples,
+count(distinct cf) AS `Case Files`,
+count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (samp:sample)--&gt;(c) 
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 MATCH (c)&lt;--(diag:diagnosis)
 WHERE s.clinical_study_designation IN ['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
-OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
 OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
 RETURN  coalesce(c.case_id, '') AS `Case ID` ,
         coalesce(s.clinical_study_designation, '') AS `Study Code` ,
         coalesce(s.clinical_study_type, '') AS  `Study Type`,
         coalesce(demo.breed, '') AS Breed ,
         coalesce(diag.disease_term, '') AS Diagnosis ,
         coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-        coalesce(co.cohort_description, '') AS `Cohort`</t>
+  coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`
+order by c.case_id asc
+limit 100</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
@@ -88,8 +118,8 @@
  WITH DISTINCT samp AS samp, c, demo, diag
 RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
         coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(demo.breed,'') AS Breed,
+        coalesce(diag.disease_term,'') AS Diagnosis, 
         coalesce(samp.sample_site, '') AS `Sample Site`,
         coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
         coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
@@ -97,7 +127,39 @@
         coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
         coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
         coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(s:study)
+MATCH (s)&lt;--(c:case)&lt;--(diag:diagnosis)
+MATCH (samp:sample)--&gt;(c)
+MATCH (c)&lt;--(demo:demographic)
+MATCH (f:file)--&gt;(parent)
+WHERE s.clinical_study_designation IN ['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
+WITH
+        DISTINCT f, c, demo, diag, s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, c, demo, diag, s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+        WITH
+        f,  c, demo, diag, s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS  Format,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`
+  order by 'File Name' asc
+  limit 100</t>
   </si>
   <si>
     <t>MATCH (f:file)--&gt;(parent)
@@ -105,55 +167,33 @@
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
 MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
 WHERE s.clinical_study_designation IN['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
- WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(f.file_type, '') AS `File Type`, 
+OPTIONAL MATCH (f)--&gt;(samp:sample)
+WITH
+        DISTINCT f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+WITH
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_type, '') AS `File Type`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
         coalesce(labels(parent)[0], '') AS `Association`,
         coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `File Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(s:study)
-MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
-WITH DISTINCT f, s
-RETURN 
-  coalesce(f.file_name, '') AS `File Name`,
-  coalesce(f.file_type, '') AS `File Type`,
-  coalesce("study", '') AS `Association`,
-  coalesce(f.file_description, '') AS `Description`,
-  coalesce(f.file_format, '') AS `File Format`,
-  coalesce(f.file_size, '') AS `Size`,
-  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>TC01_Canine_StudyNCATSCOP01-Breed_PrimDiseaseSite_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_Canine_StudyNCATSCOP01-Breed_PrimDiseaseSite_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)
-MATCH (demo:demographic) 
-MATCH (diag:diagnosis)
-MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
-OPTIONAL MATCH (s)&lt;-[:member_of]-(c:case),(s:study)
-OPTIONAL MATCH (c)&lt;-[:of_case]-(samp:sample)
-OPTIONAL MATCH (f:file)-[*]-&gt;(c)
-OPTIONAL MATCH (sf:file)--&gt;(s)
-RETURN  
-count(distinct p) AS Programs,
-count(distinct s) AS Studies,
-count(distinct c) AS Cases,
-count(distinct samp) AS Samples,
-count(distinct f) AS `Case Files`,
-count(distinct sf) AS `Study Files`</t>
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis
+        order by f.file_name asc
+        limit 100</t>
   </si>
 </sst>
 </file>
@@ -534,7 +574,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -569,16 +609,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="273.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -586,16 +626,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="181.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -603,16 +643,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="278.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -620,16 +660,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
NCATS Multifilter combination testcases- 1-70 fixed
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_StudyNCATSCOP01-Breed_PrimDiseaseSite.xlsx
+++ b/InputFiles/TC01_Canine_StudyNCATSCOP01-Breed_PrimDiseaseSite.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0502\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C65FE38-21C6-4B66-99BB-55F292DAC36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4677716F-6C35-4379-BCE7-A8607D67A2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -63,26 +63,6 @@
     <t>StudyFilesTab</t>
   </si>
   <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-MATCH (c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-        coalesce(co.cohort_description, '') AS `Cohort`</t>
-  </si>
-  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
 WHERE s.clinical_study_designation IN['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
  WITH DISTINCT samp AS samp, c, demo, diag
@@ -98,38 +78,6 @@
         coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
         coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
         coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
- WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(f.file_type, '') AS `File Type`, 
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `File Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(s:study)
-MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
-WITH DISTINCT f, s
-RETURN 
-  coalesce(f.file_name, '') AS `File Name`,
-  coalesce(f.file_type, '') AS `File Type`,
-  coalesce("study", '') AS `Association`,
-  coalesce(f.file_description, '') AS `Description`,
-  coalesce(f.file_format, '') AS `File Format`,
-  coalesce(f.file_size, '') AS `Size`,
-  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
   <si>
     <t>TC01_Canine_StudyNCATSCOP01-Breed_PrimDiseaseSite_Neo4jData.xlsx</t>
@@ -154,6 +102,96 @@
 count(distinct samp) AS Samples,
 count(distinct f) AS `Case Files`,
 count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(s:study)
+MATCH (s)&lt;--(c:case)&lt;--(diag:diagnosis)
+MATCH (r:registration)--&gt;(c)
+MATCH (c)&lt;--(demo:demographic)
+WHERE s.clinical_study_designation IN ['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
+WITH
+        DISTINCT f, c, demo, diag, s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, c, demo, diag, s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+        WITH
+        f,  c, demo, diag, s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS  Format,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`
+  order by 'File Name' asc
+  limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+OPTIONAL MATCH (c)--&gt;(ci:canine_individual)
+WITH DISTINCT c, s, demo, diag, co, ci,demo.patient_age_at_enrollment AS age, demo.weight as weight
+WHERE s.clinical_study_designation IN ['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
+RETURN  coalesce(c.case_id, '') AS `Case ID` ,
+        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
+        coalesce(s.clinical_study_type, '') AS  `Study Type`,
+        coalesce(demo.breed, '') AS Breed ,
+        coalesce(diag.disease_term, '') AS Diagnosis ,
+        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
+  coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`
+order by c.case_id asc
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)-[*]-&gt;(c:case)
+MATCH (f)--&gt;(parent)
+OPTIONAL MATCH (f)--&gt;(samp:sample)
+OPTIONAL MATCH (p:program)&lt;--(s:study)&lt;--(c)
+OPTIONAL MATCH (c)&lt;--(demo:demographic)
+OPTIONAL MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (c)--&gt;(ci:canine_individual)
+WITH 
+    f, c, parent, samp, p, s, demo, diag, ci
+WHERE s.clinical_study_designation IN ['NCATS-COP01'] and demo.breed in ['Beagle','Boxer']and diag.disease_term in ['T Cell Lymphoma'] and diag.primary_disease_site in ['Lymph Node']
+WITH 
+    DISTINCT f, c, parent, samp, p, s, demo, diag,
+    toInteger(floor(log(f.file_size)/log(1024))) as i,
+    ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+    2 as precision
+WITH
+    DISTINCT f, c, parent, samp, p, s, demo, diag,
+    f.file_size /(1024^i) AS value,
+    10^precision AS factor,
+    units[i] as unit
+WITH 
+    DISTINCT f, c, parent, samp, p, s, demo, diag, unit,
+    round(factor * value)/factor AS size
+RETURN
+    coalesce(f.file_name, '') AS `File Name`,
+    coalesce(f.file_format, '') AS `Format`,
+    coalesce(f.file_type, '') AS `File Type`,
+    CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+    coalesce(labels(parent)[0], '') AS `Association`,
+    coalesce(f.file_description, '') AS `Description`,
+    coalesce(samp.sample_id, '') AS `Sample ID`,
+    coalesce(c.case_id, '') AS `Case ID`,
+    coalesce(demo.breed,'') AS Breed ,
+    coalesce(diag.disease_term,'') AS Diagnosis
+    ORDER BY f.file_name asc
+     limit 100</t>
   </si>
 </sst>
 </file>
@@ -534,7 +572,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -569,16 +607,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="273.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -586,16 +624,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="181.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -603,16 +641,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="278.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -620,16 +658,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>